<commit_message>
Fixed save function to .xlsx / .pkl
</commit_message>
<xml_diff>
--- a/data/generated/excel/vehicles_by_line.xlsx
+++ b/data/generated/excel/vehicles_by_line.xlsx
@@ -450,7 +450,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B3" t="n">
         <v>3</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B5" t="n">
         <v>5</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>176</v>
+        <v>45</v>
       </c>
       <c r="B6" t="n">
         <v>8</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="B8" t="n">
         <v>10</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B11" t="n">
         <v>14</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="B14" t="n">
         <v>18</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B18" t="n">
         <v>22</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="B19" t="n">
         <v>24</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" t="n">
         <v>44</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B21" t="n">
         <v>49</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>157</v>
+        <v>49</v>
       </c>
       <c r="B22" t="n">
         <v>50</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B24" t="n">
         <v>72</v>

</xml_diff>

<commit_message>
Zmian a webscrappera na pryztanki w dwire strony
</commit_message>
<xml_diff>
--- a/data/generated/excel/vehicles_by_line.xlsx
+++ b/data/generated/excel/vehicles_by_line.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,7 +442,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="B3" t="n">
         <v>3</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" t="n">
         <v>5</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="B6" t="n">
         <v>8</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>70</v>
+        <v>189</v>
       </c>
       <c r="B7" t="n">
         <v>9</v>
@@ -490,7 +490,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B8" t="n">
         <v>10</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" t="n">
         <v>11</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" t="n">
         <v>13</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="B11" t="n">
         <v>14</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>16</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B13" t="n">
         <v>17</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B14" t="n">
         <v>18</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B15" t="n">
         <v>19</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B16" t="n">
         <v>20</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B18" t="n">
         <v>22</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B19" t="n">
         <v>24</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B21" t="n">
         <v>49</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="B22" t="n">
         <v>50</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="n">
         <v>52</v>
@@ -618,17 +618,25 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B25" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B26" t="n">
         <v>72</v>
       </c>
     </row>

</xml_diff>